<commit_message>
feat(scrapper): save in a xlsx
</commit_message>
<xml_diff>
--- a/influencers.xlsx
+++ b/influencers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -22,175 +22,229 @@
     <t>Followers</t>
   </si>
   <si>
-    <t>Super_papa</t>
-  </si>
-  <si>
-    <t>8776</t>
-  </si>
-  <si>
-    <t>Aiva.ru</t>
-  </si>
-  <si>
-    <t>13752</t>
-  </si>
-  <si>
-    <t>Тугеза</t>
-  </si>
-  <si>
-    <t>5397</t>
-  </si>
-  <si>
-    <t>vika_lifestyle</t>
-  </si>
-  <si>
-    <t>10803</t>
-  </si>
-  <si>
-    <t>markovatl</t>
-  </si>
-  <si>
-    <t>44123</t>
-  </si>
-  <si>
-    <t>Show</t>
-  </si>
-  <si>
-    <t>33801</t>
-  </si>
-  <si>
-    <t>Настя</t>
-  </si>
-  <si>
-    <t>4901</t>
-  </si>
-  <si>
-    <t>Пушман</t>
-  </si>
-  <si>
-    <t>44061</t>
-  </si>
-  <si>
-    <t>Papasha_live</t>
-  </si>
-  <si>
-    <t>17214</t>
-  </si>
-  <si>
-    <t>Мышка</t>
-  </si>
-  <si>
-    <t>20616</t>
-  </si>
-  <si>
-    <t>VLOG</t>
-  </si>
-  <si>
-    <t>7559</t>
-  </si>
-  <si>
-    <t>АНЮТКА-МАЛЮТКА</t>
-  </si>
-  <si>
-    <t>3585</t>
-  </si>
-  <si>
-    <t>Fox</t>
-  </si>
-  <si>
-    <t>22979</t>
-  </si>
-  <si>
-    <t>Kasparyants</t>
-  </si>
-  <si>
-    <t>40966</t>
-  </si>
-  <si>
-    <t>Konasova</t>
-  </si>
-  <si>
-    <t>28373</t>
-  </si>
-  <si>
-    <t>Kids</t>
-  </si>
-  <si>
-    <t>3163</t>
-  </si>
-  <si>
-    <t>Гигагог</t>
-  </si>
-  <si>
-    <t>3626</t>
-  </si>
-  <si>
-    <t>ЗЕМЛЕ</t>
-  </si>
-  <si>
-    <t>17323</t>
-  </si>
-  <si>
-    <t>Бровченко</t>
+    <t>Клубный Сервис</t>
+  </si>
+  <si>
+    <t>137171</t>
+  </si>
+  <si>
+    <t>За рулем</t>
+  </si>
+  <si>
+    <t>46230</t>
+  </si>
+  <si>
+    <t>Дмитрий Пучков</t>
+  </si>
+  <si>
+    <t>485385</t>
+  </si>
+  <si>
+    <t>Automps</t>
+  </si>
+  <si>
+    <t>29012</t>
+  </si>
+  <si>
+    <t>Lowvert</t>
+  </si>
+  <si>
+    <t>7679</t>
+  </si>
+  <si>
+    <t>Ильдар Авто-Подбор</t>
+  </si>
+  <si>
+    <t>419128</t>
+  </si>
+  <si>
+    <t>Игорь БУРЦЕВ  /  АВТО</t>
+  </si>
+  <si>
+    <t>5649</t>
+  </si>
+  <si>
+    <t>Rozetked</t>
+  </si>
+  <si>
+    <t>24222</t>
+  </si>
+  <si>
+    <t>DimaViper</t>
+  </si>
+  <si>
+    <t>14337</t>
+  </si>
+  <si>
+    <t>kalinka auto</t>
+  </si>
+  <si>
+    <t>1151</t>
+  </si>
+  <si>
+    <t>Тимофей из Китая</t>
+  </si>
+  <si>
+    <t>520</t>
+  </si>
+  <si>
+    <t>Большой тест-драйв</t>
+  </si>
+  <si>
+    <t>11387</t>
+  </si>
+  <si>
+    <t>Denis МЕХАНИК</t>
+  </si>
+  <si>
+    <t>36156</t>
+  </si>
+  <si>
+    <t>Жизнь Виа</t>
+  </si>
+  <si>
+    <t>32273</t>
+  </si>
+  <si>
+    <t>Погнали!</t>
+  </si>
+  <si>
+    <t>57101</t>
+  </si>
+  <si>
+    <t>Большое путешествие</t>
+  </si>
+  <si>
+    <t>6086</t>
+  </si>
+  <si>
+    <t>Axmatea</t>
+  </si>
+  <si>
+    <t>25615</t>
+  </si>
+  <si>
+    <t>nari_man007</t>
+  </si>
+  <si>
+    <t>44376</t>
+  </si>
+  <si>
+    <t>"Та сторона" с Валентиной Осокиной</t>
+  </si>
+  <si>
+    <t>17435</t>
+  </si>
+  <si>
+    <t>Александр Кондрашов</t>
+  </si>
+  <si>
+    <t>18646</t>
+  </si>
+  <si>
+    <t>Maria OMG</t>
+  </si>
+  <si>
+    <t>7002</t>
+  </si>
+  <si>
+    <t>gus_mi</t>
+  </si>
+  <si>
+    <t>21438</t>
+  </si>
+  <si>
+    <t>Лютые Походники</t>
+  </si>
+  <si>
+    <t>4294</t>
+  </si>
+  <si>
+    <t>Стас Ай, Как Просто!</t>
+  </si>
+  <si>
+    <t>260813</t>
+  </si>
+  <si>
+    <t>Double Bubble</t>
+  </si>
+  <si>
+    <t>539477</t>
+  </si>
+  <si>
+    <t>Деревенька под утёсом</t>
+  </si>
+  <si>
+    <t>20851</t>
+  </si>
+  <si>
+    <t>Юлия Пушман</t>
+  </si>
+  <si>
+    <t>44067</t>
+  </si>
+  <si>
+    <t>Семья Бровченко</t>
   </si>
   <si>
     <t>6718</t>
   </si>
   <si>
-    <t>TV</t>
-  </si>
-  <si>
-    <t>14693</t>
-  </si>
-  <si>
-    <t>DDD</t>
-  </si>
-  <si>
-    <t>3988</t>
-  </si>
-  <si>
-    <t>Me</t>
-  </si>
-  <si>
-    <t>3365</t>
-  </si>
-  <si>
-    <t>belka_podelka</t>
-  </si>
-  <si>
-    <t>32284</t>
-  </si>
-  <si>
-    <t>26208</t>
-  </si>
-  <si>
-    <t>Марк&amp;Глебас</t>
-  </si>
-  <si>
-    <t>4019</t>
-  </si>
-  <si>
-    <t>Potapova_blog</t>
-  </si>
-  <si>
-    <t>7475</t>
-  </si>
-  <si>
-    <t>Buslova</t>
-  </si>
-  <si>
-    <t>5005</t>
-  </si>
-  <si>
-    <t>Valynha</t>
-  </si>
-  <si>
-    <t>25863</t>
-  </si>
-  <si>
-    <t>SURPRISE</t>
-  </si>
-  <si>
-    <t>1692</t>
+    <t>Katya Buslova</t>
+  </si>
+  <si>
+    <t>5007</t>
+  </si>
+  <si>
+    <t>Big Big Family in the USA</t>
+  </si>
+  <si>
+    <t>743</t>
+  </si>
+  <si>
+    <t>Karina Kasparyants</t>
+  </si>
+  <si>
+    <t>40969</t>
+  </si>
+  <si>
+    <t>40970</t>
+  </si>
+  <si>
+    <t>Манюнин Дом</t>
+  </si>
+  <si>
+    <t>31981</t>
+  </si>
+  <si>
+    <t>INMYROOM</t>
+  </si>
+  <si>
+    <t>17766</t>
+  </si>
+  <si>
+    <t>ANTI-AGE</t>
+  </si>
+  <si>
+    <t>22387</t>
+  </si>
+  <si>
+    <t>Иванова Наука</t>
+  </si>
+  <si>
+    <t>6985</t>
+  </si>
+  <si>
+    <t>Другая История</t>
+  </si>
+  <si>
+    <t>24249</t>
+  </si>
+  <si>
+    <t>Наизнанку</t>
+  </si>
+  <si>
+    <t>38061</t>
   </si>
 </sst>
 </file>
@@ -566,202 +620,298 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
         <v>58</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>